<commit_message>
various updates onP Part 1.3 and Part 1.4
</commit_message>
<xml_diff>
--- a/Assignment_01/01_02/Results_IA_01-02.xlsx
+++ b/Assignment_01/01_02/Results_IA_01-02.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felixwaldschock/Documents/gits/Chalmers_TME286_IntelligentAgents/Assignment_01/01_02/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BBFA094-FEA5-184C-8748-952F38E0F39D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA7C3232-7025-EB49-BA34-48CF139D2EE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25760" yWindow="8220" windowWidth="25760" windowHeight="18420" xr2:uid="{014E1AE5-F580-D24D-86C5-4306381C3A56}"/>
+    <workbookView xWindow="-25760" yWindow="8220" windowWidth="25760" windowHeight="16980" xr2:uid="{014E1AE5-F580-D24D-86C5-4306381C3A56}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>Word</t>
   </si>
@@ -105,6 +105,36 @@
   </si>
   <si>
     <t>or</t>
+  </si>
+  <si>
+    <t>Negative</t>
+  </si>
+  <si>
+    <t>Correct classified:</t>
+  </si>
+  <si>
+    <t>Flasly Classified</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> before boarding , the terrible customer service people at the gate made people check their bags even though there was an excessive amount of space in overhead compartments . with their terrible rate of baggage loss , this has ruined my flight and others .</t>
+  </si>
+  <si>
+    <t>london to delhi . an excellent service and experience . this was my first time travelling with ai and i was amazed with service from ground staff to onboard . i'm looking forward flying with ai again in future .</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> london heathrow to algiers on an old 767 . cabin crew are simply not professional food wasn't appealing and toilets were filthy .</t>
+  </si>
+  <si>
+    <t>terrible service . mean and unkind employees . left me waiting 46 minutes to find a wheelchair . doesn’t have enough staff to operate wheelchair or check everyone in . horrible food .</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>Validation</t>
   </si>
 </sst>
 </file>
@@ -114,7 +144,7 @@
   <numFmts count="1">
     <numFmt numFmtId="169" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -124,6 +154,12 @@
     </font>
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Helvetica"/>
       <family val="2"/>
@@ -149,13 +185,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,21 +507,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8135804-3A59-5941-9DCE-65E32A44C753}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="3"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -497,8 +541,17 @@
       <c r="D2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -508,8 +561,20 @@
       <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D3" s="2">
+        <v>-7.3593803962037798</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="I3">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -519,8 +584,11 @@
       <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D4" s="2">
+        <v>-6.9300100000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -530,8 +598,11 @@
       <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D5" s="2">
+        <v>-6.1804800000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -541,8 +612,11 @@
       <c r="C6" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D6" s="2">
+        <v>-5.7775400000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -552,8 +626,11 @@
       <c r="C7" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D7" s="2">
+        <v>-5.08507</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -563,8 +640,11 @@
       <c r="C8" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D8" s="2">
+        <v>-5.0396939999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -574,8 +654,11 @@
       <c r="C9" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D9" s="2">
+        <v>-4.8361999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -585,8 +668,11 @@
       <c r="C10" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D10" s="2">
+        <v>-4.5254000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -596,8 +682,11 @@
       <c r="C11" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D11" s="2">
+        <v>-4.3102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -607,27 +696,51 @@
       <c r="C12" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D12" s="2">
+        <v>-5.2602000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C13" s="1"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D13" s="2"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="C17" s="1"/>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C19" t="s">
-        <v>14</v>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>